<commit_message>
Fix chain-id in A5-A6 and Complete A7-A20
</commit_message>
<xml_diff>
--- a/Exclusive048/evidence.xlsx
+++ b/Exclusive048/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11325" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11325" tabRatio="614" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="155">
   <si>
     <t>TeamName</t>
   </si>
@@ -81,21 +81,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -187,6 +172,342 @@
   </si>
   <si>
     <t>426E654143A090C0C6140ED0412BB993C0DC0341ADB84EB55639A5A5102382D0</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; s </t>
+  </si>
+  <si>
+    <t>s --(1)--&gt; j</t>
+  </si>
+  <si>
+    <t> j --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
+  </si>
+  <si>
+    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; u </t>
+  </si>
+  <si>
+    <t>u --(1)--&gt; o</t>
+  </si>
+  <si>
+    <t>o --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>ibc/84EFE646043023F7F446F982B03C80A066C745558D75820FDA3ACD64DDD97734</t>
+  </si>
+  <si>
+    <t>ibc/698B9551F9BF42D5B1B40C3F1A4D30DAF30BB5F1DFF3DFA550FA1E4608629104</t>
+  </si>
+  <si>
+    <t>ibc/59399DE993384EABA96794F81A545C4252C7DCA2FE2DBC926C717E9E3D12B21C</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; s</t>
+  </si>
+  <si>
+    <t> s --(1)--&gt; j</t>
+  </si>
+  <si>
+    <t>j --(1)--&gt; u</t>
+  </si>
+  <si>
+    <t>u --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>ibc/F87D334DD62D764256FEF4B2A830E0A7B28A8CCE95E30CA23C7E2DAC44948461</t>
+  </si>
+  <si>
+    <t>s --(1)--&gt; o</t>
+  </si>
+  <si>
+    <t>o --(1)--&gt; j</t>
+  </si>
+  <si>
+    <t>ibc/FAC32942183234F018BC237A494231116EDFE525909FF2F01F667F455D19CB6C</t>
+  </si>
+  <si>
+    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-44/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
+  </si>
+  <si>
+    <t>ibc/37A875F9C358B490F7771694C7F9BEBD020FDEF69E07A30EBD9B5C7F0AFC318D</t>
+  </si>
+  <si>
+    <t>7430E7B0D17EAB930C7999FCBB9868333726B279920B578C6CEC56379B809C2E</t>
+  </si>
+  <si>
+    <t>Stage 2</t>
+  </si>
+  <si>
+    <t>excnft006</t>
+  </si>
+  <si>
+    <t>4ACF1C20DFF8B3F6F1AF49DDC693C62718DC763B5B5104595CAF4FEE929D5D07</t>
+  </si>
+  <si>
+    <t>excnft007</t>
+  </si>
+  <si>
+    <t>excnft008</t>
+  </si>
+  <si>
+    <t>excnft009</t>
+  </si>
+  <si>
+    <t>AA810240AF9BE27040387C4085ACEDCF1A112B741D4C3DECF9B0BEA41732FAFA</t>
+  </si>
+  <si>
+    <t>4FFACA7F6798EDA3DC064986DA9568DB24D98CBE50F85FEC324CD5598385336D</t>
+  </si>
+  <si>
+    <t> s --(1)--&gt; j </t>
+  </si>
+  <si>
+    <t> j --(1)--&gt; u </t>
+  </si>
+  <si>
+    <t>o --(1)--&gt; s</t>
+  </si>
+  <si>
+    <t>s --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>ibc/6F974D8BC175A163D5FE18FD5DA263C07164E6F93CE6DB7E0A5370AD0187E663</t>
+  </si>
+  <si>
+    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-41/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
+  </si>
+  <si>
+    <t>ibc/AACF1ECB4DDB33B6DE6A6E768AE64249680684D3D1ED9BE98877AD547213916B</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; o</t>
+  </si>
+  <si>
+    <t>s --(1)--&gt; u</t>
+  </si>
+  <si>
+    <t>j --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>ibc/F155F9B9F3F9D5FEEB640340CE61C12754344DC47C1E0A5D361154DE542FCAFD</t>
+  </si>
+  <si>
+    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-24/excprotocol001</t>
+  </si>
+  <si>
+    <t>ibc/5DC841D55BE412CB2DEDDFCB9F395370E8EA59FB32824D47F63284970FEF238A</t>
+  </si>
+  <si>
+    <t>ibc/12A7211CEC444BE79138637332B73F631250D5F75E3D8910483A4D8FDF2F376B</t>
+  </si>
+  <si>
+    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-41/nft-transfer/channel-6/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-24/excprotocol001</t>
+  </si>
+  <si>
+    <t>ibc/9922819D336D16531E12DFA6731DD34CC611E2627D932B1DFBA1472DDC5BA9DA</t>
+  </si>
+  <si>
+    <t>ibc/F4EBE09806BF850BCD1D32B7BA75202E6E375550FF14C600C4E5A4335787A71D</t>
+  </si>
+  <si>
+    <t>u --(1)--&gt; s </t>
+  </si>
+  <si>
+    <t>s --(2)--&gt; i</t>
+  </si>
+  <si>
+    <t>5B58DD9C883C7329D1A436358A79998BEFD89942E66117D5BCA705FA53EA9FCF</t>
+  </si>
+  <si>
+    <t>20A2C5A7255E7EF9A4219DFC9CE0794655C136C97669E8FF1870480E5F04A31C</t>
+  </si>
+  <si>
+    <t>C4F783A4348E811A60EB41C393C41ADCEEAE65383D184661EBDEC86E6D5ED901</t>
+  </si>
+  <si>
+    <t>9B605C65F28A1000D46E3C06DA50FEC50F4959105E39CCD984717A8651F5E2DA</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; u</t>
+  </si>
+  <si>
+    <t>o --(1)--&gt; u </t>
+  </si>
+  <si>
+    <t> u --(2)--&gt; i</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>30589798533C024256FE64D8521C269E4337924B5CBDFEBAC768856EE976828A</t>
+  </si>
+  <si>
+    <t>BD5B99EC631C3CBEE948D3B9B39E8326545DE24A482B000715802545B8CB58E7</t>
+  </si>
+  <si>
+    <t>F02630434BEB6B869770078133BF2C38DEAF59397A0080662F25E13B1CEFD546</t>
+  </si>
+  <si>
+    <t>3D9771E510919F083A523D038B62551E192BA03496B4E661C9F98AABF22E6897</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; j </t>
+  </si>
+  <si>
+    <t>u --(1)--&gt; j</t>
+  </si>
+  <si>
+    <t> j --(2)--&gt; i</t>
+  </si>
+  <si>
+    <t>j --(1)--&gt; s</t>
+  </si>
+  <si>
+    <t>j --(2)--&gt; i</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>897CF08011954A7CC246B2EFF3688A52B70840B1B63DE818B9923BC136850F47</t>
+  </si>
+  <si>
+    <t>excnft010</t>
+  </si>
+  <si>
+    <t>04F2B2CEF48D9ED0A5217F4E44E32598177B7D6EAC17CF469144CAFD69550B8C</t>
+  </si>
+  <si>
+    <t>excnft011</t>
+  </si>
+  <si>
+    <t>5FB08093A44D359FCC58EA28FA0D9CDC27E9B0ED0470336C0425DA2963C0F2BE</t>
+  </si>
+  <si>
+    <t>excnft012</t>
+  </si>
+  <si>
+    <t>excnft013</t>
+  </si>
+  <si>
+    <t>994704C3DB2C13271748820CB11BAD9EBA62F2F6696B613BCBB2BFEECA991462</t>
+  </si>
+  <si>
+    <t>excnft014</t>
+  </si>
+  <si>
+    <t>891873369084744974D492A6E4DAE0450B365D3AB0B175611F5B5B4C5B72EDD9</t>
+  </si>
+  <si>
+    <t>excnft015</t>
+  </si>
+  <si>
+    <t>E99A18741A66CD466F4DBD4E03DD7305BD1938BC86A58A7751653898541B9559</t>
+  </si>
+  <si>
+    <t>AB8BA2A0CAB228F5670BCDCCCAFCBFC49C82BD07E9AB2185420E41F9A73D1AC8</t>
+  </si>
+  <si>
+    <t>91476CD97B6E8C7BE44A3408AAA544F5180390E91DEDBE73E4FD9ECBA2EC1F10</t>
+  </si>
+  <si>
+    <t>FEDA611844F8EFA305C5514C7DA9520192576D275E3908850753E313A8E857D5</t>
+  </si>
+  <si>
+    <t>BF09CB38BA2E199FE3D5D3803A06F8A9F9CBA443791E794C441649401D7D74BF</t>
+  </si>
+  <si>
+    <t>B94D1CCEA5794EFEFC834A25008A819D3977CC4DBA63AEB139A0D1BAEE950970</t>
+  </si>
+  <si>
+    <t>807A1706C08EC68BF898A4046CC6892FA641615887981CCEDF748629B880ADE9</t>
+  </si>
+  <si>
+    <t>D5157939CBCBCE62368451F675C8E528291ED05A99D97C3CFB05659D958CE7B2</t>
+  </si>
+  <si>
+    <t>2754F3D7121A71CB4D6915DEB2F483593BC7F920CAA043C5192132496C29F573</t>
+  </si>
+  <si>
+    <t> j --(1)--&gt; s</t>
+  </si>
+  <si>
+    <t>B9921E227DFDE6577B6A61E11C43E396AB2FB9B1EC5F10B95475B53D24A39599</t>
+  </si>
+  <si>
+    <t>8F77CB4D65D56D57068F11A6A724D432FA2E3F747315EF6C1E343F5B83584768</t>
+  </si>
+  <si>
+    <t>488E37D192718CCA4A5FF8073B39FE0A8D2E575EE70D861E50B7D271CCADC55F</t>
+  </si>
+  <si>
+    <t>D99C8530364D81AD04AB476BAEAA6347CBFDFD60A5EEB46BEE3C6D80B8F1A63D</t>
+  </si>
+  <si>
+    <t>o --(1)--&gt; u</t>
+  </si>
+  <si>
+    <t>396686D0EA297CAFA928DE79E62CB8984B33A90318C8751C3790478D475E56B7</t>
+  </si>
+  <si>
+    <t>2C5893C8D408459E05A22D59B10B782BA3B7C91156953C37DFC1082630C4ADDF</t>
+  </si>
+  <si>
+    <t>79D3FE7B113A4F3C37B809CE46F5716105DA6B6D0F40BA1DC6BB0F5C53ABD756</t>
+  </si>
+  <si>
+    <t>7115B455A75EC6765C3C0170B8A3C6A69F1D7239CC670FB35559FD310457F202</t>
+  </si>
+  <si>
+    <t>s --(1)--&gt; j </t>
+  </si>
+  <si>
+    <t>u --(1)--&gt; j </t>
+  </si>
+  <si>
+    <t>o --(1)--&gt; s </t>
+  </si>
+  <si>
+    <t>0C7D080CEAFA0F34C6760FCDA633EAD40A35143F073B4AD88EE501A05EC95A9F</t>
+  </si>
+  <si>
+    <t>F3597B314FF4BE96A7654C78A9C62796B1D7E879DA57C0AF2E6278B404DF4B6E</t>
+  </si>
+  <si>
+    <t>183701F5AE0C1FE04E667A23DE38ED609A49D60FA79EEADAD72DAFBF5757CDC1</t>
+  </si>
+  <si>
+    <t>F5AF397534D94232D5FF0221277E222B6FC37ADA682DACBF21601EA8C3520FEF</t>
+  </si>
+  <si>
+    <t>B235AC18A3E7D72C37CD72F987B0ED389A9966966DEE0ED4FFAA1A4B317BC8F4</t>
+  </si>
+  <si>
+    <t>41A61919BEFD228058C9030BD4D94F4F59007BD3C2C0423204497847FEC7A8B4</t>
+  </si>
+  <si>
+    <t>8DA510708FE4C97F471D8967F7F0AEEF7F5372572196ECFBB030C1F09DAA4C34</t>
+  </si>
+  <si>
+    <t>AA433DB7B2DD280CDB67207469BB5F3CD8B888029587DAAA92A11C7066085D0A</t>
+  </si>
+  <si>
+    <t>301B9567C9353C4AF95E4B0DEAF250D59508E46C77C537F73D96C98936869641</t>
+  </si>
+  <si>
+    <t>CFE527D1C05E3A43A2F3BC60FD7D74E16C50634E12BA65311C70AF4B4EC9E7BE</t>
+  </si>
+  <si>
+    <t>654BB5F9A670942A026BD430AE8BF6FA9171268C618C1F58B1A94D7F0C079744</t>
+  </si>
+  <si>
+    <t>23F60302AC28BEC14E7706DB9F28E5A3B580813471AEF9EA681A9A55D9FB8D49</t>
   </si>
 </sst>
 </file>
@@ -240,11 +561,10 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <charset val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -279,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -293,10 +613,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -643,7 +963,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -685,28 +1005,28 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -717,16 +1037,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="107.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -734,12 +1056,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>34</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -750,16 +1108,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="93.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -767,12 +1127,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>36</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -783,16 +1179,18 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="121" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -800,12 +1198,70 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -816,16 +1272,18 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="113" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -833,12 +1291,70 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>68</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -849,16 +1365,19 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -866,23 +1385,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -892,16 +1440,19 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -909,23 +1460,55 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -935,16 +1518,18 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="86.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -952,23 +1537,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -978,16 +1592,18 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="84.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -995,23 +1611,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1021,16 +1666,18 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1038,22 +1685,48 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>133</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1064,16 +1737,19 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1081,23 +1757,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1129,10 +1835,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1143,16 +1849,19 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1160,22 +1869,70 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>145</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1186,16 +1943,19 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1203,22 +1963,70 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>151</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1242,12 +2050,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1277,12 +2085,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1312,12 +2120,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1347,12 +2155,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1367,20 +2175,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1391,59 +2199,199 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>40</v>
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1457,13 +2405,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="84.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1484,16 +2432,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1507,12 +2455,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1533,16 +2482,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1555,13 +2504,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="107.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1581,16 +2531,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +2554,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1630,17 +2580,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>47</v>
+      <c r="A2" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1651,16 +2601,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="86.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1668,12 +2621,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1684,18 +2663,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="86.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1703,12 +2682,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix classID(delete prefix wasm.) in A3,A5
</commit_message>
<xml_diff>
--- a/Exclusive048/evidence.xlsx
+++ b/Exclusive048/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11325" tabRatio="614" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11325" tabRatio="614" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>89EE72A97074051420FFF2FBBFC52E9C298C8C24D3FC134764330352AEEB4501</t>
   </si>
   <si>
-    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-208/excprotocol001</t>
-  </si>
-  <si>
     <t>elgafar-1</t>
   </si>
   <si>
@@ -508,13 +505,16 @@
   </si>
   <si>
     <t>23F60302AC28BEC14E7706DB9F28E5A3B580813471AEF9EA681A9A55D9FB8D49</t>
+  </si>
+  <si>
+    <t>stars1lfzq8es9uukrcx0tkyggn0hllx0xk88r7dkwhdu38qf9fx875cesk3pydz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -566,6 +566,13 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6E6B7B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -611,12 +618,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1039,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1057,47 +1064,47 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>46</v>
+      <c r="A2" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>54</v>
+        <v>33</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>57</v>
+        <v>33</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1128,47 +1135,47 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>46</v>
+      <c r="A2" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>54</v>
+        <v>35</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>59</v>
+        <v>35</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>60</v>
+        <v>35</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>45</v>
+        <v>35</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1182,7 +1189,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1199,69 +1206,69 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>46</v>
+      <c r="A2" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>54</v>
+        <v>65</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>49</v>
+        <v>65</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1292,69 +1299,69 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>83</v>
+      <c r="A2" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>75</v>
+        <v>67</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>49</v>
+        <v>67</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>60</v>
+        <v>67</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>82</v>
+        <v>67</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1387,46 +1394,46 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>54</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>81</v>
+        <v>31</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1462,46 +1469,46 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>96</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1539,46 +1546,46 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>104</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>56</v>
+        <v>108</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B5" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1613,46 +1620,46 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>104</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>129</v>
-      </c>
       <c r="B5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="12" t="s">
         <v>108</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1687,46 +1694,46 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>54</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>134</v>
-      </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>76</v>
+        <v>31</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1759,51 +1766,51 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="12"/>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1871,68 +1878,68 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>54</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>140</v>
+        <v>31</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>56</v>
+        <v>108</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>141</v>
+        <v>37</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>130</v>
+        <v>108</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>76</v>
+        <v>31</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1965,68 +1972,68 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>96</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>90</v>
+        <v>37</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>154</v>
-      </c>
       <c r="B7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>57</v>
+        <v>37</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2200,13 +2207,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2217,7 +2224,7 @@
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2228,170 +2235,170 @@
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>34</v>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>36</v>
+      <c r="C6" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>66</v>
+      <c r="C7" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>68</v>
+      <c r="C8" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>69</v>
+      <c r="C9" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>70</v>
+      <c r="C10" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>111</v>
+      <c r="C11" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>113</v>
+      <c r="C12" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>115</v>
+      <c r="C13" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>116</v>
+      <c r="C14" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>118</v>
+      <c r="C15" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>120</v>
+      <c r="C16" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2412,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2434,14 +2441,14 @@
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2482,16 +2489,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2505,7 +2512,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2531,16 +2538,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2580,17 +2587,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>42</v>
+      <c r="A2" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2603,8 +2610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2623,36 +2630,36 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>43</v>
+      <c r="C2" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>47</v>
+      <c r="A3" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>44</v>
+      <c r="C3" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>58</v>
+      <c r="A4" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>45</v>
+      <c r="C4" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2684,35 +2691,35 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>48</v>
+      <c r="C2" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>52</v>
+      <c r="A3" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>49</v>
+      <c r="C3" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>51</v>
+      <c r="A4" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>50</v>
+      <c r="C4" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix format answers for A7-A20
</commit_message>
<xml_diff>
--- a/Exclusive048/evidence.xlsx
+++ b/Exclusive048/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11325" tabRatio="614" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11325" tabRatio="614" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
   <si>
     <t>TeamName</t>
   </si>
@@ -171,66 +171,12 @@
     <t>426E654143A090C0C6140ED0412BB993C0DC0341ADB84EB55639A5A5102382D0</t>
   </si>
   <si>
-    <t>i --(1)--&gt; s </t>
-  </si>
-  <si>
-    <t>s --(1)--&gt; j</t>
-  </si>
-  <si>
-    <t> j --(1)--&gt; i</t>
-  </si>
-  <si>
-    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
-  </si>
-  <si>
-    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
-  </si>
-  <si>
-    <t>i --(1)--&gt; u </t>
-  </si>
-  <si>
-    <t>u --(1)--&gt; o</t>
-  </si>
-  <si>
-    <t>o --(1)--&gt; i</t>
-  </si>
-  <si>
     <t>ibc/84EFE646043023F7F446F982B03C80A066C745558D75820FDA3ACD64DDD97734</t>
   </si>
   <si>
-    <t>ibc/698B9551F9BF42D5B1B40C3F1A4D30DAF30BB5F1DFF3DFA550FA1E4608629104</t>
-  </si>
-  <si>
-    <t>ibc/59399DE993384EABA96794F81A545C4252C7DCA2FE2DBC926C717E9E3D12B21C</t>
-  </si>
-  <si>
-    <t>i --(1)--&gt; s</t>
-  </si>
-  <si>
-    <t> s --(1)--&gt; j</t>
-  </si>
-  <si>
-    <t>j --(1)--&gt; u</t>
-  </si>
-  <si>
-    <t>u --(1)--&gt; i</t>
-  </si>
-  <si>
     <t>ibc/F87D334DD62D764256FEF4B2A830E0A7B28A8CCE95E30CA23C7E2DAC44948461</t>
   </si>
   <si>
-    <t>s --(1)--&gt; o</t>
-  </si>
-  <si>
-    <t>o --(1)--&gt; j</t>
-  </si>
-  <si>
-    <t>ibc/FAC32942183234F018BC237A494231116EDFE525909FF2F01F667F455D19CB6C</t>
-  </si>
-  <si>
-    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-44/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
-  </si>
-  <si>
     <t>ibc/37A875F9C358B490F7771694C7F9BEBD020FDEF69E07A30EBD9B5C7F0AFC318D</t>
   </si>
   <si>
@@ -261,63 +207,15 @@
     <t>4FFACA7F6798EDA3DC064986DA9568DB24D98CBE50F85FEC324CD5598385336D</t>
   </si>
   <si>
-    <t> s --(1)--&gt; j </t>
-  </si>
-  <si>
-    <t> j --(1)--&gt; u </t>
-  </si>
-  <si>
-    <t>o --(1)--&gt; s</t>
-  </si>
-  <si>
-    <t>s --(1)--&gt; i</t>
-  </si>
-  <si>
-    <t>ibc/6F974D8BC175A163D5FE18FD5DA263C07164E6F93CE6DB7E0A5370AD0187E663</t>
-  </si>
-  <si>
-    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-41/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/excprotocol001</t>
-  </si>
-  <si>
     <t>ibc/AACF1ECB4DDB33B6DE6A6E768AE64249680684D3D1ED9BE98877AD547213916B</t>
   </si>
   <si>
-    <t>i --(1)--&gt; o</t>
-  </si>
-  <si>
-    <t>s --(1)--&gt; u</t>
-  </si>
-  <si>
-    <t>j --(1)--&gt; i</t>
-  </si>
-  <si>
-    <t>ibc/F155F9B9F3F9D5FEEB640340CE61C12754344DC47C1E0A5D361154DE542FCAFD</t>
-  </si>
-  <si>
-    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-24/excprotocol001</t>
-  </si>
-  <si>
-    <t>ibc/5DC841D55BE412CB2DEDDFCB9F395370E8EA59FB32824D47F63284970FEF238A</t>
-  </si>
-  <si>
-    <t>ibc/12A7211CEC444BE79138637332B73F631250D5F75E3D8910483A4D8FDF2F376B</t>
-  </si>
-  <si>
-    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-41/nft-transfer/channel-6/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-24/excprotocol001</t>
-  </si>
-  <si>
     <t>ibc/9922819D336D16531E12DFA6731DD34CC611E2627D932B1DFBA1472DDC5BA9DA</t>
   </si>
   <si>
     <t>ibc/F4EBE09806BF850BCD1D32B7BA75202E6E375550FF14C600C4E5A4335787A71D</t>
   </si>
   <si>
-    <t>u --(1)--&gt; s </t>
-  </si>
-  <si>
-    <t>s --(2)--&gt; i</t>
-  </si>
-  <si>
     <t>5B58DD9C883C7329D1A436358A79998BEFD89942E66117D5BCA705FA53EA9FCF</t>
   </si>
   <si>
@@ -330,15 +228,6 @@
     <t>9B605C65F28A1000D46E3C06DA50FEC50F4959105E39CCD984717A8651F5E2DA</t>
   </si>
   <si>
-    <t>i --(1)--&gt; u</t>
-  </si>
-  <si>
-    <t>o --(1)--&gt; u </t>
-  </si>
-  <si>
-    <t> u --(2)--&gt; i</t>
-  </si>
-  <si>
     <t>gon-flixnet-1</t>
   </si>
   <si>
@@ -354,21 +243,6 @@
     <t>3D9771E510919F083A523D038B62551E192BA03496B4E661C9F98AABF22E6897</t>
   </si>
   <si>
-    <t>i --(1)--&gt; j </t>
-  </si>
-  <si>
-    <t>u --(1)--&gt; j</t>
-  </si>
-  <si>
-    <t> j --(2)--&gt; i</t>
-  </si>
-  <si>
-    <t>j --(1)--&gt; s</t>
-  </si>
-  <si>
-    <t>j --(2)--&gt; i</t>
-  </si>
-  <si>
     <t>uni-6</t>
   </si>
   <si>
@@ -432,9 +306,6 @@
     <t>2754F3D7121A71CB4D6915DEB2F483593BC7F920CAA043C5192132496C29F573</t>
   </si>
   <si>
-    <t> j --(1)--&gt; s</t>
-  </si>
-  <si>
     <t>B9921E227DFDE6577B6A61E11C43E396AB2FB9B1EC5F10B95475B53D24A39599</t>
   </si>
   <si>
@@ -447,9 +318,6 @@
     <t>D99C8530364D81AD04AB476BAEAA6347CBFDFD60A5EEB46BEE3C6D80B8F1A63D</t>
   </si>
   <si>
-    <t>o --(1)--&gt; u</t>
-  </si>
-  <si>
     <t>396686D0EA297CAFA928DE79E62CB8984B33A90318C8751C3790478D475E56B7</t>
   </si>
   <si>
@@ -460,15 +328,6 @@
   </si>
   <si>
     <t>7115B455A75EC6765C3C0170B8A3C6A69F1D7239CC670FB35559FD310457F202</t>
-  </si>
-  <si>
-    <t>s --(1)--&gt; j </t>
-  </si>
-  <si>
-    <t>u --(1)--&gt; j </t>
-  </si>
-  <si>
-    <t>o --(1)--&gt; s </t>
   </si>
   <si>
     <t>0C7D080CEAFA0F34C6760FCDA633EAD40A35143F073B4AD88EE501A05EC95A9F</t>
@@ -1044,15 +903,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="107.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -1064,48 +923,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>45</v>
+      <c r="A2" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1115,15 +939,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="93.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -1135,48 +959,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>45</v>
+      <c r="A2" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1186,15 +975,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="121" customWidth="1"/>
+    <col min="1" max="1" width="76" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -1206,70 +995,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>45</v>
+      <c r="A2" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>75</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1279,15 +1011,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="113" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -1299,70 +1031,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>82</v>
+      <c r="A2" t="s">
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>81</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1375,7 +1050,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1394,47 +1069,39 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>53</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>89</v>
-      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>90</v>
-      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
@@ -1450,7 +1117,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1469,47 +1136,39 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>95</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>48</v>
-      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>96</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>97</v>
-      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="7"/>
@@ -1528,7 +1187,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1546,47 +1205,39 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>103</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>55</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>105</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
@@ -1602,7 +1253,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1620,47 +1271,39 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>103</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>106</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>107</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
@@ -1676,7 +1319,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1694,47 +1337,39 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>53</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>129</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="C5" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1747,7 +1382,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1766,50 +1401,42 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>79</v>
-      </c>
+      <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>134</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>48</v>
-      </c>
+      <c r="C4" s="11"/>
       <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>49</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="11"/>
     </row>
   </sheetData>
@@ -1859,7 +1486,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1878,69 +1505,57 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>53</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>139</v>
-      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>55</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>140</v>
-      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>129</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="C7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1952,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1972,69 +1587,57 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>95</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>89</v>
-      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>141</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="C7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2263,142 +1866,142 @@
     </row>
     <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2442,7 +2045,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>26</v>
@@ -2541,7 +2144,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>26</v>
@@ -2608,10 +2211,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2620,7 +2223,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2628,39 +2231,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>45</v>
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2670,15 +2248,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -2690,37 +2268,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>38</v>
+      <c r="A2" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>49</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>